<commit_message>
Update Oracle - e20 to own ga.xlsx
</commit_message>
<xml_diff>
--- a/source/databricks/calculation_engine/tests/features/given_an_energy_calculation/when_exchange_sends_to_own_ga/Oracle - e20 to own ga.xlsx
+++ b/source/databricks/calculation_engine/tests/features/given_an_energy_calculation/when_exchange_sends_to_own_ga/Oracle - e20 to own ga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\opengeh-wholesale\source\databricks\calculation_engine\tests\features\given_an_energy_calculation\when_exchange_sends_to_own_ga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B62A6BB-58E6-49A5-A656-DD1ECD5E8757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59681D7C-2D11-4F86-BE61-3913A669191C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="51420" windowHeight="21100" xr2:uid="{B26405EC-4681-4CC9-BF80-F87B3459AD72}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="114">
   <si>
     <t>energy_supplier_id</t>
   </si>
@@ -464,7 +464,7 @@
     <t>180000001500000001</t>
   </si>
   <si>
-    <t>production</t>
+    <t>flex_consumption</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1410,7 @@
   <dimension ref="A1:CN400"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:H25"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1605,15 +1605,15 @@
       </c>
       <c r="AE2" s="27" t="str" cm="1">
         <f t="array" ref="AE2">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(AE28:AE41,AE28:AE41 &lt;&gt; "")))</f>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="AF2" s="27" t="str" cm="1">
         <f t="array" ref="AF2">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(AF28:AF40,AF28:AF40 &lt;&gt; "")))</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="AG2" s="27" t="str">
         <f>IF(B$2="production","E18",IF($B$2="flex_consumption","D01","E02"))</f>
-        <v>E18</v>
+        <v>D01</v>
       </c>
       <c r="AH2" s="27" t="str" cm="1">
         <f t="array" ref="AH2">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.VSTACK(_xlfn._xlws.FILTER(TableDay1[from_ga],TableDay1[from_ga] &lt;&gt; ""),_xlfn._xlws.FILTER(TableDay1[to_ga],TableDay1[to_ga] &lt;&gt; ""))))</f>
@@ -2045,24 +2045,24 @@
       </c>
       <c r="T10" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U10,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="U10" s="26" t="str">
         <f>IF(AE$2=0,"",AE$2)</f>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="V10" s="20">
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[es_id],U10,IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT1H")/4</f>
-        <v>0</v>
+        <v>0.27775</v>
       </c>
       <c r="W10" s="19">
         <f>V10</f>
-        <v>0</v>
+        <v>0.27775</v>
       </c>
       <c r="X10" s="19"/>
       <c r="Y10" s="23">
         <f t="shared" ref="Y10:Y33" si="1">ROUND(W10, 3)</f>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="Z10" s="27"/>
       <c r="AA10" s="24"/>
@@ -2100,27 +2100,27 @@
       </c>
       <c r="T11" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U11,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="U11" s="26" t="str">
         <f t="shared" ref="U11:V13" si="2">U$10</f>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="V11" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.27775</v>
       </c>
       <c r="W11" s="19">
         <f>X11+W10</f>
-        <v>0</v>
+        <v>0.27749999999999997</v>
       </c>
       <c r="X11" s="19">
         <f>V11-Y10</f>
-        <v>0</v>
+        <v>-2.5000000000002798E-4</v>
       </c>
       <c r="Y11" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="Z11" s="27"/>
       <c r="AA11" s="24"/>
@@ -2175,27 +2175,27 @@
       </c>
       <c r="T12" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U12,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="U12" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="V12" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.27775</v>
       </c>
       <c r="W12" s="19">
         <f>X12+W11</f>
-        <v>0</v>
+        <v>0.27724999999999994</v>
       </c>
       <c r="X12" s="19">
         <f>V12-Y11</f>
-        <v>0</v>
+        <v>-2.5000000000002798E-4</v>
       </c>
       <c r="Y12" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="Z12" s="27"/>
       <c r="AA12" s="24"/>
@@ -2240,27 +2240,27 @@
       </c>
       <c r="T13" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U13,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="U13" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="V13" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.27775</v>
       </c>
       <c r="W13" s="19">
         <f>X13+W12</f>
-        <v>0</v>
+        <v>0.27799999999999991</v>
       </c>
       <c r="X13" s="19">
         <f>V13-Y12</f>
-        <v>0</v>
+        <v>7.4999999999997291E-4</v>
       </c>
       <c r="Y13" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="Z13" s="27"/>
       <c r="AA13" s="24"/>
@@ -2537,9 +2537,7 @@
       <c r="D16" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>91</v>
-      </c>
+      <c r="E16" s="11"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="41"/>
@@ -3018,7 +3016,7 @@
     <row r="20" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" s="44" t="str">
         <f>CONCATENATE(B2,"_per_",B1)</f>
-        <v>production_per_ga_brp_es</v>
+        <v>flex_consumption_per_ga_brp_es</v>
       </c>
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
@@ -3267,11 +3265,11 @@
       <c r="A22" s="2"/>
       <c r="B22" s="16" t="str">
         <f>IF(AND(F22&lt;&gt;"null",F22&lt;&gt;""),IF(F22=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G22&lt;&gt;"null",G22&lt;&gt;""),IF(G22=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E22=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C22" s="16" t="str">
         <f>IF(AND(F22&lt;&gt;"null",F22&lt;&gt;""),IF(F22=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G22&lt;&gt;"null",G22&lt;&gt;""),IF(G22=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E22=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D22" s="15" t="s">
         <v>74</v>
@@ -3282,27 +3280,27 @@
       </c>
       <c r="F22" s="31" t="str">
         <f>IF(B$1="ga",IF(E22="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G22="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="G22" s="31" t="str">
         <f>IF(B$1="ga",IF(E22="","","null"),IF(B$1="ga_es",IF(F22="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F22="","",INDEX(TableDay1[brp_id],MATCH(F22,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ref="H22:H45" ca="1" si="5">SUBSTITUTE(IF(E22="","",I22+J22+K22),",",".")</f>
-        <v>1.278</v>
+        <v>0.278</v>
       </c>
       <c r="I22" s="9">
         <f>SUMIFS(Y$10:Y$33,IF(OR(B$1="ga_es",B$1="ga_brp_es"),U$10:U$33,IF(B$1="ga_brp",T$10:T$33,S$10:S$33)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F22,IF(B$1="ga_brp",G22,E22)),R$10:R$33,D22)</f>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="J22" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D22,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D22,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F22,IF(B$1="ga_brp",G22,E22)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="9">
         <f t="shared" ref="K22:K45" si="6">IF(AND(C22="skmp",B$2="production"),VLOOKUP(D22,D$78:H$81,5,FALSE),IF(AND(B22="glmp",B$2="flex_consumption"),VLOOKUP(D22,D$72:H$75,5,FALSE),0))</f>
-        <v>0.27800000000000002</v>
+        <v>0</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -3409,11 +3407,11 @@
     <row r="23" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B23" s="16" t="str">
         <f>IF(AND(F23&lt;&gt;"null",F23&lt;&gt;""),IF(F23=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G23&lt;&gt;"null",G23&lt;&gt;""),IF(G23=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E23=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C23" s="16" t="str">
         <f>IF(AND(F23&lt;&gt;"null",F23&lt;&gt;""),IF(F23=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G23&lt;&gt;"null",G23&lt;&gt;""),IF(G23=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E23=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D23" s="15" t="s">
         <v>75</v>
@@ -3424,11 +3422,11 @@
       </c>
       <c r="F23" s="31" t="str">
         <f>IF(B$1="ga",IF(E23="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G23="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="G23" s="31" t="str">
         <f>IF(B$1="ga",IF(E23="","","null"),IF(B$1="ga_es",IF(F23="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F23="","",INDEX(TableDay1[brp_id],MATCH(F23,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3436,7 +3434,7 @@
       </c>
       <c r="I23" s="9">
         <f t="shared" ref="I23:I45" si="8">SUMIFS(Y$10:Y$33,IF(OR(B$1="ga_es",B$1="ga_brp_es"),U$10:U$33,IF(B$1="ga_brp",T$10:T$33,S$10:S$33)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F23,IF(B$1="ga_brp",G23,E23)),R$10:R$33,D23)</f>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="J23" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D23,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D23,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F23,IF(B$1="ga_brp",G23,E23)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
@@ -3444,7 +3442,7 @@
       </c>
       <c r="K23" s="9">
         <f t="shared" si="6"/>
-        <v>0.27800000000000002</v>
+        <v>0</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -3554,11 +3552,11 @@
     <row r="24" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B24" s="16" t="str">
         <f>IF(AND(F24&lt;&gt;"null",F24&lt;&gt;""),IF(F24=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G24&lt;&gt;"null",G24&lt;&gt;""),IF(G24=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E24=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C24" s="16" t="str">
         <f>IF(AND(F24&lt;&gt;"null",F24&lt;&gt;""),IF(F24=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G24&lt;&gt;"null",G24&lt;&gt;""),IF(G24=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E24=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D24" s="15" t="s">
         <v>76</v>
@@ -3569,11 +3567,11 @@
       </c>
       <c r="F24" s="31" t="str">
         <f>IF(B$1="ga",IF(E24="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G24="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="G24" s="31" t="str">
         <f>IF(B$1="ga",IF(E24="","","null"),IF(B$1="ga_es",IF(F24="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F24="","",INDEX(TableDay1[brp_id],MATCH(F24,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3581,7 +3579,7 @@
       </c>
       <c r="I24" s="9">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="J24" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D24,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D24,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F24,IF(B$1="ga_brp",G24,E24)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
@@ -3589,7 +3587,7 @@
       </c>
       <c r="K24" s="9">
         <f t="shared" si="6"/>
-        <v>0.27700000000000002</v>
+        <v>0</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -3702,11 +3700,11 @@
     <row r="25" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B25" s="16" t="str">
         <f>IF(AND(F25&lt;&gt;"null",F25&lt;&gt;""),IF(F25=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G25&lt;&gt;"null",G25&lt;&gt;""),IF(G25=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E25=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C25" s="16" t="str">
         <f>IF(AND(F25&lt;&gt;"null",F25&lt;&gt;""),IF(F25=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G25&lt;&gt;"null",G25&lt;&gt;""),IF(G25=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E25=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D25" s="15" t="s">
         <v>77</v>
@@ -3717,11 +3715,11 @@
       </c>
       <c r="F25" s="31" t="str">
         <f>IF(B$1="ga",IF(E25="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G25="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>1000000000000</v>
       </c>
       <c r="G25" s="31" t="str">
         <f>IF(B$1="ga",IF(E25="","","null"),IF(B$1="ga_es",IF(F25="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F25="","",INDEX(TableDay1[brp_id],MATCH(F25,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>1100000000000</v>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3729,7 +3727,7 @@
       </c>
       <c r="I25" s="9">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="J25" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D25,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D25,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F25,IF(B$1="ga_brp",G25,E25)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
@@ -3737,7 +3735,7 @@
       </c>
       <c r="K25" s="9">
         <f t="shared" si="6"/>
-        <v>0.27800000000000002</v>
+        <v>0</v>
       </c>
       <c r="L25" s="37"/>
       <c r="M25" s="2"/>
@@ -4073,11 +4071,11 @@
       <c r="AD27" s="36"/>
       <c r="AE27" s="36" t="str">
         <f>_xlfn.CONCAT("Energy suppliers for "&amp;B2)</f>
-        <v>Energy suppliers for production</v>
+        <v>Energy suppliers for flex_consumption</v>
       </c>
       <c r="AF27" s="36" t="str">
         <f>_xlfn.CONCAT("Balance responsibles for "&amp;B2)</f>
-        <v>Balance responsibles for production</v>
+        <v>Balance responsibles for flex_consumption</v>
       </c>
       <c r="AG27" s="36"/>
       <c r="AH27" s="36"/>
@@ -4223,12 +4221,12 @@
       <c r="AC28" s="2"/>
       <c r="AD28" s="36"/>
       <c r="AE28" s="36" t="str" cm="1">
-        <f t="array" ref="AE28">IFERROR(IF($B$2="production",INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE13)*(TableDay1[type]="E18"),""),,9),INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE13)*(TableDay1[settlement_method]=AG$2),""),,9)),"")</f>
-        <v/>
+        <f t="array" ref="AE28">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE13)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE13)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <v>1000000000000</v>
       </c>
       <c r="AF28" s="36" t="str" cm="1">
         <f t="array" ref="AF28">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF13)*(TableDay1[type]=$AG$2),""),,10)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF13)*(TableDay1[settlement_method]=AG$2),""),,10))),"")</f>
-        <v/>
+        <v>1100000000000</v>
       </c>
       <c r="AG28" s="36"/>
       <c r="AH28" s="36"/>
@@ -4368,9 +4366,13 @@
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
       <c r="AD29" s="36"/>
+      <c r="AE29" s="36" t="str" cm="1">
+        <f t="array" ref="AE29">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE14)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE14)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <v/>
+      </c>
       <c r="AF29" s="36" t="str" cm="1">
         <f t="array" ref="AF29">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF14)*(TableDay1[type]=$AG$2),""),,10)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF14)*(TableDay1[settlement_method]=AG$2),""),,10))),"")</f>
-        <v>2200000000000</v>
+        <v/>
       </c>
       <c r="AG29" s="36"/>
       <c r="AH29" s="36"/>
@@ -4508,8 +4510,8 @@
       <c r="AC30" s="2"/>
       <c r="AD30" s="36"/>
       <c r="AE30" s="36" t="str" cm="1">
-        <f t="array" ref="AE30">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE14)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE14)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
-        <v>3000000000000</v>
+        <f t="array" ref="AE30">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE15)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE15)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <v/>
       </c>
       <c r="AF30" s="36" t="str" cm="1">
         <f t="array" ref="AF30">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF15)*(TableDay1[type]=$AG$2),""),,10)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF15)*(TableDay1[settlement_method]=AG$2),""),,10))),"")</f>
@@ -4654,7 +4656,7 @@
       <c r="AC31" s="2"/>
       <c r="AD31" s="36"/>
       <c r="AE31" s="36" t="str" cm="1">
-        <f t="array" ref="AE31">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE15)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE15)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE31">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE16)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE16)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF31" s="36" t="str" cm="1">
@@ -4800,7 +4802,7 @@
       <c r="AC32" s="2"/>
       <c r="AD32" s="36"/>
       <c r="AE32" s="36" t="str" cm="1">
-        <f t="array" ref="AE32">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE16)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE16)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE32">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE17)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE17)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF32" s="36" t="str" cm="1">
@@ -4946,7 +4948,7 @@
       <c r="AC33" s="2"/>
       <c r="AD33" s="36"/>
       <c r="AE33" s="36" t="str" cm="1">
-        <f t="array" ref="AE33">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE17)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE17)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE33">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE18)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE18)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF33" s="36" t="str" cm="1">
@@ -5069,7 +5071,7 @@
       <c r="AC34" s="2"/>
       <c r="AD34" s="36"/>
       <c r="AE34" s="36" t="str" cm="1">
-        <f t="array" ref="AE34">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE18)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE18)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE34">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE19)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE19)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF34" s="36" t="str" cm="1">
@@ -5203,7 +5205,7 @@
       <c r="AC35" s="2"/>
       <c r="AD35" s="36"/>
       <c r="AE35" s="36" t="str" cm="1">
-        <f t="array" ref="AE35">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE19)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE19)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE35">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE20)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE20)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF35" s="36" t="str" cm="1">
@@ -5339,7 +5341,7 @@
       <c r="AC36" s="2"/>
       <c r="AD36" s="36"/>
       <c r="AE36" s="36" t="str" cm="1">
-        <f t="array" ref="AE36">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE20)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE20)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE36">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE21)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE21)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF36" s="36" t="str" cm="1">
@@ -5476,7 +5478,7 @@
       <c r="AC37" s="2"/>
       <c r="AD37" s="36"/>
       <c r="AE37" s="36" t="str" cm="1">
-        <f t="array" ref="AE37">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE21)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE21)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE37">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE22)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE22)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF37" s="36" t="str" cm="1">
@@ -5616,7 +5618,7 @@
       <c r="AC38" s="2"/>
       <c r="AD38" s="36"/>
       <c r="AE38" s="36" t="str" cm="1">
-        <f t="array" ref="AE38">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE22)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE22)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE38">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE23)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE23)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF38" s="36" t="str" cm="1">
@@ -5756,7 +5758,7 @@
       <c r="AC39" s="2"/>
       <c r="AD39" s="36"/>
       <c r="AE39" s="36" t="str" cm="1">
-        <f t="array" ref="AE39">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE23)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE23)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE39">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE24)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE24)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF39" s="36" t="str" cm="1">
@@ -5896,7 +5898,7 @@
       <c r="AC40" s="2"/>
       <c r="AD40" s="36"/>
       <c r="AE40" s="36" t="str" cm="1">
-        <f t="array" ref="AE40">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE24)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE24)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE40">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE25)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE25)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF40" s="36" t="str" cm="1">
@@ -6030,7 +6032,7 @@
       <c r="AC41" s="2"/>
       <c r="AD41" s="36"/>
       <c r="AE41" s="36" t="str" cm="1">
-        <f t="array" ref="AE41">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE25)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE25)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE41">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE26)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE26)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF41" s="36" t="str" cm="1">
@@ -6166,7 +6168,7 @@
       <c r="AC42" s="2"/>
       <c r="AD42" s="36"/>
       <c r="AE42" s="36" t="str" cm="1">
-        <f t="array" ref="AE42">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE26)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE26)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
+        <f t="array" ref="AE42">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE27)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE27)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
         <v/>
       </c>
       <c r="AF42" s="36" t="str" cm="1">
@@ -6302,14 +6304,8 @@
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
       <c r="AD43" s="36"/>
-      <c r="AE43" s="36" t="str" cm="1">
-        <f t="array" ref="AE43">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE27)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE27)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
-        <v/>
-      </c>
-      <c r="AF43" s="36" t="str" cm="1">
-        <f t="array" ref="AF43">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF28)*(TableDay1[type]=$AG$2),""),,10)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF28)*(TableDay1[settlement_method]=AG$2),""),,10))),"")</f>
-        <v/>
-      </c>
+      <c r="AE43" s="36"/>
+      <c r="AF43" s="36"/>
       <c r="AG43" s="36"/>
       <c r="AH43" s="36"/>
       <c r="AI43" s="2"/>
@@ -40492,23 +40488,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="17d0a144-7218-432a-80c1-1473a2ac0f84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010083C51B3A6863BB4086AAB9D84DF721A3" ma:contentTypeVersion="9" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="9d92303bd8f83ad3ed572bd327ba273d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="17d0a144-7218-432a-80c1-1473a2ac0f84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e272e23039cec0e41a69c8e3deb1ff81" ns3:_="">
     <xsd:import namespace="17d0a144-7218-432a-80c1-1473a2ac0f84"/>
@@ -40684,31 +40663,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51BD707-A63C-4C12-A5D3-024A5FAE9E8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="17d0a144-7218-432a-80c1-1473a2ac0f84"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4F67E43-074E-4C0F-B170-E53BCA717C8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="17d0a144-7218-432a-80c1-1473a2ac0f84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE2584E-1495-47FC-B560-4437F91C3A10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40724,4 +40696,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4F67E43-074E-4C0F-B170-E53BCA717C8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51BD707-A63C-4C12-A5D3-024A5FAE9E8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="17d0a144-7218-432a-80c1-1473a2ac0f84"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>